<commit_message>
+kategorie słownictwa +lola runs - scenariusz +wortschatzübungen
</commit_message>
<xml_diff>
--- a/nv-verbindungen/n-v-verb.xlsx
+++ b/nv-verbindungen/n-v-verb.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="15000" windowHeight="7995"/>
+    <workbookView xWindow="247" yWindow="123" windowWidth="15003" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
     <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="247">
   <si>
     <t>Mut haben</t>
   </si>
@@ -745,6 +745,18 @@
   </si>
   <si>
     <t>bać się [czegoś]</t>
+  </si>
+  <si>
+    <t>Mitleid haben mit D</t>
+  </si>
+  <si>
+    <t>współczuć [komuś]</t>
+  </si>
+  <si>
+    <t>Hass haben auf A</t>
+  </si>
+  <si>
+    <t>żywić nienawiść do [kogoś/czegoś]</t>
   </si>
 </sst>
 </file>
@@ -1086,20 +1098,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:G123"/>
+  <dimension ref="B1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94:XFD123"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.75"/>
   <cols>
-    <col min="1" max="1" width="1.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.625" customWidth="1"/>
-    <col min="6" max="6" width="41.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7">
@@ -2224,6 +2236,22 @@
         <v>128</v>
       </c>
       <c r="G123" s="10"/>
+    </row>
+    <row r="124" spans="2:7">
+      <c r="B124" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F124" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="125" spans="2:7">
+      <c r="B125" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F125" s="4" t="s">
+        <v>246</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="B1:G123">
@@ -2240,7 +2268,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2252,7 +2280,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>